<commit_message>
cleaned y2 labels csv file
</commit_message>
<xml_diff>
--- a/data/labels_y2.xlsx
+++ b/data/labels_y2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiayangzhang/Library/CloudStorage/GoogleDrive-jiayang.zhang@icloud.com/My Drive/nlp-physicseducation/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/jz2319_ic_ac_uk/Documents/year4/nlp-physicseducation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C1CFFD-A8A6-9F44-81C7-D9E31450E44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{79C1CFFD-A8A6-9F44-81C7-D9E31450E44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00680EF4-A3BC-DC4C-B50A-FF0487DA9802}"/>
   <bookViews>
-    <workbookView xWindow="14040" yWindow="500" windowWidth="22640" windowHeight="21100" xr2:uid="{8B954240-007D-1145-B888-E015D178DECC}"/>
+    <workbookView xWindow="16240" yWindow="3480" windowWidth="22640" windowHeight="21100" xr2:uid="{8B954240-007D-1145-B888-E015D178DECC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -86,12 +86,6 @@
     <t>2ndINT_MOX979_Redacted</t>
   </si>
   <si>
-    <t>2ndINT_NGT6557_Redacted</t>
-  </si>
-  <si>
-    <t>2ndINT_NHZ838_Redacted</t>
-  </si>
-  <si>
     <t>NONE</t>
   </si>
   <si>
@@ -182,12 +176,6 @@
     <t>2ndINT_XUQ367_Redacted</t>
   </si>
   <si>
-    <t>2ndINT_YMU516_Redacted</t>
-  </si>
-  <si>
-    <t>2ndINT_YzI659_Redacted</t>
-  </si>
-  <si>
     <t>2ndINT_AAN562_Redacted</t>
   </si>
   <si>
@@ -318,6 +306,18 @@
   </si>
   <si>
     <t>2ndINT_GXI055_Redacted</t>
+  </si>
+  <si>
+    <t>2ndINT_NGT657_Redacted</t>
+  </si>
+  <si>
+    <t>2ndINT_NHZ839_Redacted</t>
+  </si>
+  <si>
+    <t>2ndINT_YMJ516_Redacted</t>
+  </si>
+  <si>
+    <t>2ndINT_YZI659_Redacted</t>
   </si>
 </sst>
 </file>
@@ -701,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39BE24EA-C5F2-404F-95D1-44D0E5D7E8DD}">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,18 +714,18 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -737,7 +737,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -749,10 +749,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
@@ -761,19 +761,19 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
@@ -785,10 +785,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>2</v>
@@ -797,7 +797,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
@@ -809,19 +809,19 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
@@ -833,7 +833,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>1</v>
@@ -845,19 +845,19 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>1</v>
@@ -869,7 +869,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
@@ -881,7 +881,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>9</v>
@@ -893,7 +893,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>4</v>
@@ -905,7 +905,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>9</v>
@@ -917,7 +917,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>9</v>
@@ -929,7 +929,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>13</v>
@@ -941,7 +941,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>9</v>
@@ -953,7 +953,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>9</v>
@@ -965,7 +965,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>9</v>
@@ -977,7 +977,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>9</v>
@@ -989,19 +989,19 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>9</v>
@@ -1013,10 +1013,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>7</v>
@@ -1025,7 +1025,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>9</v>
@@ -1037,7 +1037,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>9</v>
@@ -1049,7 +1049,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>4</v>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>9</v>
@@ -1073,10 +1073,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>7</v>
@@ -1085,19 +1085,19 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>4</v>
@@ -1109,7 +1109,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>1</v>
@@ -1121,7 +1121,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>13</v>
@@ -1133,10 +1133,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>5</v>
@@ -1145,19 +1145,19 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>9</v>
@@ -1169,7 +1169,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>1</v>
@@ -1181,7 +1181,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>9</v>
@@ -1193,7 +1193,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>1</v>
@@ -1205,7 +1205,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>1</v>
@@ -1318,7 +1318,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="B52" t="s">
         <v>4</v>
@@ -1329,18 +1329,18 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="B53" t="s">
         <v>4</v>
       </c>
       <c r="C53" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B54" t="s">
         <v>13</v>
@@ -1351,7 +1351,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B55" t="s">
         <v>4</v>
@@ -1362,10 +1362,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B56" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C56" t="s">
         <v>2</v>
@@ -1373,7 +1373,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B57" t="s">
         <v>9</v>
@@ -1384,21 +1384,21 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B58" t="s">
         <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B59" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
@@ -1406,7 +1406,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B60" t="s">
         <v>4</v>
@@ -1417,10 +1417,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B61" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
@@ -1428,7 +1428,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B62" t="s">
         <v>4</v>
@@ -1439,7 +1439,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B63" t="s">
         <v>4</v>
@@ -1450,7 +1450,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B64" t="s">
         <v>4</v>
@@ -1461,10 +1461,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B65" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
@@ -1472,7 +1472,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B66" t="s">
         <v>4</v>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B67" t="s">
         <v>4</v>
@@ -1494,21 +1494,21 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B68" t="s">
         <v>9</v>
       </c>
       <c r="C68" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B69" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C69" t="s">
         <v>2</v>
@@ -1516,7 +1516,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B70" t="s">
         <v>9</v>
@@ -1527,7 +1527,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B71" t="s">
         <v>9</v>
@@ -1538,10 +1538,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B72" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C72" t="s">
         <v>2</v>
@@ -1549,7 +1549,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B73" t="s">
         <v>4</v>
@@ -1560,7 +1560,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B74" t="s">
         <v>9</v>
@@ -1571,7 +1571,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B75" t="s">
         <v>9</v>
@@ -1582,7 +1582,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B76" t="s">
         <v>4</v>
@@ -1593,7 +1593,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B77" t="s">
         <v>4</v>
@@ -1604,21 +1604,21 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B78" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C78" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B79" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>5</v>
@@ -1626,10 +1626,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B80" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C80" t="s">
         <v>2</v>
@@ -1637,7 +1637,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B81" t="s">
         <v>4</v>
@@ -1648,7 +1648,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B82" t="s">
         <v>4</v>
@@ -1659,7 +1659,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="B83" t="s">
         <v>9</v>
@@ -1670,7 +1670,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="B84" t="s">
         <v>9</v>
@@ -1680,6 +1680,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C84">
+    <sortCondition ref="A2:A84"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>